<commit_message>
template ready for download
</commit_message>
<xml_diff>
--- a/TEMPLATES/heartbeat_config_INPUT_template.xlsx
+++ b/TEMPLATES/heartbeat_config_INPUT_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/ananyak_s_philips_com/Documents/Saved Pictures/heartbeat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/ananyak_s_philips_com/Documents/Saved Pictures/heartbeat/TEMPLATES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_AD4DB114E441178AC67DF4BEEE14EB98693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6391C614-3499-4208-928C-F93FB95C0CC6}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_AD4DB114E441178AC67DF4BEEE14EB98693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2306227-A61C-4486-A609-B0C4D56070D3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>type</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>http</t>
+  </si>
+  <si>
+    <t>IPV4/V5</t>
   </si>
 </sst>
 </file>
@@ -189,6 +192,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -216,20 +233,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -243,8 +246,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F52FC1D-6E7A-4DD3-9660-3CBE9F59DBE1}" name="Table1" displayName="Table1" ref="A1:Z1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F52FC1D-6E7A-4DD3-9660-3CBE9F59DBE1}" name="Table1" displayName="Table1" ref="A1:Z1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:Z1048576" xr:uid="{6F52FC1D-6E7A-4DD3-9660-3CBE9F59DBE1}"/>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{02D7C2DF-7F19-4673-80B4-6408643A42C3}" name="type"/>
@@ -544,7 +551,7 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,12 +661,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9EB07404-8E18-41B6-B70F-960E2F7DED8A}">
           <x14:formula1>
             <xm:f>'support sheet'!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B26C9933-00BA-40B8-8DE3-59FBFE328B34}">
+          <x14:formula1>
+            <xm:f>'support sheet'!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576 F1:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -669,30 +682,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790E7915-46B5-4567-B66B-3F42207694C9}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>

</xml_diff>